<commit_message>
Day 3 - Historical FCFF & Ratios
- Added EBITDA, NOPAT, NWC, FCFF, ROIC, FCF-Margin, EBITDA-Margin & 3-yr
  revenue CAGR formulas in DCF sheet.
- Created scripts/data_fetcher.py to pull marketCap & EBITDA and write
  to Inputs
- Inputs sheet now autocalculates EV and EV/EBITDA multiple
- Updated Raw_FS to keep clean 4-year history
- Minor clean-up: .gitignore tracks *.csv debug dumps
</commit_message>
<xml_diff>
--- a/templates/DCF_Model.xlsx
+++ b/templates/DCF_Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\valuation-model\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8EFDD4-F8A1-4780-B709-41AD53DCD466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CAD313-C891-41CA-8A06-D23BF5A765EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -20,27 +20,24 @@
   </sheets>
   <definedNames>
     <definedName name="capex_pct">Inputs!$B$13</definedName>
-    <definedName name="current_price">DCF!$B$24</definedName>
+    <definedName name="current_price">DCF!$B$25</definedName>
     <definedName name="dep_pct">Inputs!$B$14</definedName>
     <definedName name="ebit_target">Inputs!$B$12</definedName>
-    <definedName name="equity_value">DCF!$B$21</definedName>
-    <definedName name="ev">DCF!$B$19</definedName>
+    <definedName name="equity_value">DCF!$B$22</definedName>
+    <definedName name="ev">DCF!$B$20</definedName>
     <definedName name="forecast_horizon">Inputs!$B$10</definedName>
-    <definedName name="implied_price">DCF!$B$23</definedName>
-    <definedName name="net_debt">DCF!$B$20</definedName>
+    <definedName name="implied_price">DCF!$B$24</definedName>
+    <definedName name="net_debt">DCF!$B$21</definedName>
     <definedName name="nwc_pct">Inputs!$B$15</definedName>
-    <definedName name="pv_fcff_total">DCF!$B$18</definedName>
+    <definedName name="pv_fcff_total">DCF!$B$19</definedName>
     <definedName name="sales_cagr">Inputs!$B$11</definedName>
-    <definedName name="shares_out">DCF!$B$22</definedName>
+    <definedName name="shares_out">DCF!$B$23</definedName>
     <definedName name="tax_rate">Inputs!$B$8</definedName>
-    <definedName name="upside_pct">DCF!$B$25</definedName>
+    <definedName name="upside_pct">DCF!$B$26</definedName>
     <definedName name="wacc">Inputs!$B$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -56,26 +53,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={FAFE5303-75CC-4400-85AB-B9AAEB311C43}</author>
-  </authors>
-  <commentList>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{FAFE5303-75CC-4400-85AB-B9AAEB311C43}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    (Cost of Equity) * Equity Weight + (Cost of Debt after tax) * Debt Weight</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t>Ticker</t>
   </si>
@@ -95,6 +74,9 @@
     <t>Risk-Free Rate</t>
   </si>
   <si>
+    <t>Pre-Tax Cost of Debt</t>
+  </si>
+  <si>
     <t>Tax Rate</t>
   </si>
   <si>
@@ -128,16 +110,115 @@
     <t>Margin of Safety %</t>
   </si>
   <si>
+    <t>WACC</t>
+  </si>
+  <si>
+    <t>Market Cap</t>
+  </si>
+  <si>
+    <t>Latest EBITDA (yfinance)</t>
+  </si>
+  <si>
+    <t>Enterprise Value</t>
+  </si>
+  <si>
+    <t>EV/EBITDA</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>ebit</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>dep_amort</t>
+  </si>
+  <si>
+    <t>capex</t>
+  </si>
+  <si>
+    <t>assets</t>
+  </si>
+  <si>
+    <t>debt</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>ap</t>
+  </si>
+  <si>
+    <t>Year-columns</t>
+  </si>
+  <si>
+    <t>2025F</t>
+  </si>
+  <si>
+    <t>2026F</t>
+  </si>
+  <si>
+    <t>2027F</t>
+  </si>
+  <si>
+    <t>2028F</t>
+  </si>
+  <si>
+    <t>2029F</t>
+  </si>
+  <si>
     <t>Revenue</t>
   </si>
   <si>
+    <t>Sales</t>
+  </si>
+  <si>
     <t>EBIT</t>
   </si>
   <si>
+    <t>EBIT Margin</t>
+  </si>
+  <si>
+    <t>NOPAT</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
     <t>Dep &amp; Amort</t>
   </si>
   <si>
-    <t>NOPAT</t>
+    <t>EBITDA</t>
+  </si>
+  <si>
+    <t>EBITDA Margin</t>
+  </si>
+  <si>
+    <t>CapEx</t>
+  </si>
+  <si>
+    <t>∆NWC</t>
   </si>
   <si>
     <t>FCFF</t>
@@ -146,71 +227,18 @@
     <t>ROIC</t>
   </si>
   <si>
+    <t>Discount Factor</t>
+  </si>
+  <si>
     <t>FCF Margin</t>
   </si>
   <si>
-    <t>Year-columns</t>
-  </si>
-  <si>
-    <t>CapEx</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>∆</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>NWC</t>
-    </r>
+    <t>PV of FCFF</t>
   </si>
   <si>
     <t>CAGRs</t>
   </si>
   <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>EBIT Margin</t>
-  </si>
-  <si>
-    <t>Tax</t>
-  </si>
-  <si>
-    <t>2025F</t>
-  </si>
-  <si>
-    <t>2026F</t>
-  </si>
-  <si>
-    <t>2027F</t>
-  </si>
-  <si>
-    <t>2028F</t>
-  </si>
-  <si>
-    <t>2029F</t>
-  </si>
-  <si>
-    <t>Discount Factor</t>
-  </si>
-  <si>
-    <t>PV of FCFF</t>
-  </si>
-  <si>
-    <t>WACC</t>
-  </si>
-  <si>
     <t>Terminal FCFF</t>
   </si>
   <si>
@@ -253,22 +281,18 @@
     <t>LT Growth (g)</t>
   </si>
   <si>
-    <t>EV/EBITDA</t>
-  </si>
-  <si>
     <t>Margin of Safety</t>
-  </si>
-  <si>
-    <t>Pre-Tax Cost of Debt</t>
-  </si>
-  <si>
-    <t>Line-Item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,###,,"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,###,,,"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,20 +310,8 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <i/>
@@ -315,6 +327,18 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -337,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -405,44 +429,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -457,13 +507,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -475,12 +518,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Lucas Duran" id="{A2646D1A-6F4F-4B1A-AF54-764AA21BEEBF}" userId="3397f29ba12d6d12" providerId="Windows Live"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -744,29 +781,22 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B19" dT="2025-07-10T17:00:52.71" personId="{A2646D1A-6F4F-4B1A-AF54-764AA21BEEBF}" id="{FAFE5303-75CC-4400-85AB-B9AAEB311C43}">
-    <text>(Cost of Equity) * Equity Weight + (Cost of Debt after tax) * Debt Weight</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -787,7 +817,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -808,11 +838,11 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -829,7 +859,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -850,7 +880,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -871,7 +901,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -892,9 +922,9 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -913,9 +943,9 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -934,11 +964,11 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="13"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -955,9 +985,9 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -976,9 +1006,9 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -997,9 +1027,9 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1018,11 +1048,11 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="13"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1039,11 +1069,11 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="14"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="13"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1060,11 +1090,11 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="13"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1081,9 +1111,9 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1102,9 +1132,9 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1123,11 +1153,11 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="13"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1144,14 +1174,11 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1">
-        <f>((B6+B4*B5)*(1-B9))+(B7*(1-B8)*B9)</f>
-        <v>0</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1168,9 +1195,13 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+    <row r="20" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="23">
+        <v>3736529010688</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1187,9 +1218,13 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+    <row r="21" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="23">
+        <v>149172994048</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1206,9 +1241,14 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+    <row r="22" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="23">
+        <f>B20+Raw_FS!B8-Raw_FS!B9</f>
+        <v>3785341010688</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1225,9 +1265,14 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+    <row r="23" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="25">
+        <f>B22/B21</f>
+        <v>25.375511397659388</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1244,8 +1289,8 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+    <row r="24" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1263,8 +1308,8 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
+    <row r="25" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1282,7 +1327,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1301,7 +1346,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1320,7 +1365,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1339,7 +1384,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1358,7 +1403,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1377,7 +1422,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1396,7 +1441,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1415,7 +1460,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1434,7 +1479,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1453,7 +1498,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1472,7 +1517,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1491,7 +1536,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1510,7 +1555,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1529,7 +1574,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1548,7 +1593,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1567,7 +1612,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1586,7 +1631,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1605,7 +1650,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1624,7 +1669,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1643,7 +1688,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1662,7 +1707,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1681,7 +1726,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1700,7 +1745,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1719,7 +1764,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1738,7 +1783,7 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1757,7 +1802,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1776,7 +1821,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1795,806 +1840,476 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A71B2FA-345D-4205-A12A-4C546D259E0F}">
-  <dimension ref="A1:I49"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
+    <row r="53" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>245122000000</v>
+      </c>
+      <c r="C2">
+        <v>211915000000</v>
+      </c>
+      <c r="D2">
+        <v>198270000000</v>
+      </c>
+      <c r="E2">
+        <v>168088000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>110722000000</v>
+      </c>
+      <c r="C3">
+        <v>91279000000</v>
+      </c>
+      <c r="D3">
+        <v>85779000000</v>
+      </c>
+      <c r="E3">
+        <v>73448000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>19651000000</v>
+      </c>
+      <c r="C4">
+        <v>16950000000</v>
+      </c>
+      <c r="D4">
+        <v>10978000000</v>
+      </c>
+      <c r="E4">
+        <v>9831000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>22287000000</v>
+      </c>
+      <c r="C5">
+        <v>13861000000</v>
+      </c>
+      <c r="D5">
+        <v>14460000000</v>
+      </c>
+      <c r="E5">
+        <v>11686000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>-44477000000</v>
+      </c>
+      <c r="C6">
+        <v>-28107000000</v>
+      </c>
+      <c r="D6">
+        <v>-23886000000</v>
+      </c>
+      <c r="E6">
+        <v>-20622000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>512163000000</v>
+      </c>
+      <c r="C7">
+        <v>411976000000</v>
+      </c>
+      <c r="D7">
+        <v>364840000000</v>
+      </c>
+      <c r="E7">
+        <v>333779000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>67127000000</v>
+      </c>
+      <c r="C8">
+        <v>59965000000</v>
+      </c>
+      <c r="D8">
+        <v>61270000000</v>
+      </c>
+      <c r="E8">
+        <v>67775000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>18315000000</v>
+      </c>
+      <c r="C9">
+        <v>34704000000</v>
+      </c>
+      <c r="D9">
+        <v>13931000000</v>
+      </c>
+      <c r="E9">
+        <v>14224000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>56924000000</v>
+      </c>
+      <c r="C10">
+        <v>48688000000</v>
+      </c>
+      <c r="D10">
+        <v>44261000000</v>
+      </c>
+      <c r="E10">
+        <v>38043000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>1246000000</v>
+      </c>
+      <c r="C11">
+        <v>2500000000</v>
+      </c>
+      <c r="D11">
+        <v>3742000000</v>
+      </c>
+      <c r="E11">
+        <v>2636000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>21996000000</v>
+      </c>
+      <c r="C12">
+        <v>18095000000</v>
+      </c>
+      <c r="D12">
+        <v>19000000000</v>
+      </c>
+      <c r="E12">
+        <v>15163000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E90302-80A9-49D4-B703-292350D04CBD}">
-  <dimension ref="A1:Q155"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Q156"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="8">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="7">
         <v>2024</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="8">
         <v>2023</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="8">
         <v>2022</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="8">
         <v>2021</v>
       </c>
-      <c r="F1" s="9">
-        <v>2020</v>
-      </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F1" s="10"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1">
+        <v>44</v>
+      </c>
+      <c r="B2" s="23">
         <f>Raw_FS!B$2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
+        <v>245122000000</v>
+      </c>
+      <c r="C2" s="23">
         <f>Raw_FS!C$2</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
+        <v>211915000000</v>
+      </c>
+      <c r="D2" s="23">
         <f>Raw_FS!D$2</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
+        <v>198270000000</v>
+      </c>
+      <c r="E2" s="23">
         <f>Raw_FS!E$2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <f>Raw_FS!F$2</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="1">
+        <v>168088000000</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="I2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="23">
         <f>$B2*(1+sales_cagr)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
+        <v>245122000000</v>
+      </c>
+      <c r="K2" s="23">
         <f>J$2*(1+sales_cagr)</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
+        <v>245122000000</v>
+      </c>
+      <c r="L2" s="23">
         <f>K$2*(1+sales_cagr)</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
+        <v>245122000000</v>
+      </c>
+      <c r="M2" s="23">
         <f>L$2*(1+sales_cagr)</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
+        <v>245122000000</v>
+      </c>
+      <c r="N2" s="23">
         <f>M$2*(1+sales_cagr)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+        <v>245122000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1">
-        <f>Raw_FS!B$6</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <f>Raw_FS!C$6</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <f>Raw_FS!D$6</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <f>Raw_FS!E$6</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <f>Raw_FS!F$6</f>
-        <v>0</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B3" s="23">
+        <f>Raw_FS!B$3</f>
+        <v>110722000000</v>
+      </c>
+      <c r="C3" s="23">
+        <f>Raw_FS!C$3</f>
+        <v>91279000000</v>
+      </c>
+      <c r="D3" s="23">
+        <f>Raw_FS!D$3</f>
+        <v>85779000000</v>
+      </c>
+      <c r="E3" s="23">
+        <f>Raw_FS!E$3</f>
+        <v>73448000000</v>
+      </c>
+      <c r="F3" s="17"/>
       <c r="I3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="1">
+        <v>47</v>
+      </c>
+      <c r="J3" s="23">
         <f>ebit_target</f>
         <v>0</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="23">
         <f>ebit_target</f>
         <v>0</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="23">
         <f>ebit_target</f>
         <v>0</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="23">
         <f>ebit_target</f>
         <v>0</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="23">
         <f>ebit_target</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="22">
         <f>Inputs!$B$8</f>
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="22">
         <f>Inputs!$B$8</f>
         <v>0</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="22">
         <f>Inputs!$B$8</f>
         <v>0</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="22">
         <f>Inputs!$B$8</f>
         <v>0</v>
       </c>
-      <c r="F4" s="1">
-        <f>Inputs!$B$8</f>
-        <v>0</v>
-      </c>
+      <c r="F4" s="17"/>
       <c r="I4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1">
+        <v>46</v>
+      </c>
+      <c r="J4" s="23">
         <f>J2*J3</f>
         <v>0</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" ref="K4:N4" si="0">K2*K3</f>
+      <c r="K4" s="23">
+        <f>K2*K3</f>
         <v>0</v>
       </c>
-      <c r="L4" s="1">
-        <f t="shared" si="0"/>
+      <c r="L4" s="23">
+        <f>L2*L3</f>
         <v>0</v>
       </c>
-      <c r="M4" s="1">
-        <f t="shared" si="0"/>
+      <c r="M4" s="23">
+        <f>M2*M3</f>
         <v>0</v>
       </c>
-      <c r="N4" s="1">
-        <f t="shared" si="0"/>
+      <c r="N4" s="23">
+        <f>N2*N3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1">
+        <v>48</v>
+      </c>
+      <c r="B5" s="23">
         <f>B3*(1-B4)</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" ref="C5:F5" si="1">C3*(1-C4)</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>110722000000</v>
+      </c>
+      <c r="C5" s="23">
+        <f>C3*(1-C4)</f>
+        <v>91279000000</v>
+      </c>
+      <c r="D5" s="23">
+        <f>D3*(1-D4)</f>
+        <v>85779000000</v>
+      </c>
+      <c r="E5" s="23">
+        <f>E3*(1-E4)</f>
+        <v>73448000000</v>
+      </c>
+      <c r="F5" s="17"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="1">
+        <v>49</v>
+      </c>
+      <c r="J5" s="23">
         <f>J4*tax_rate</f>
         <v>0</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="23">
         <f>K4*tax_rate</f>
         <v>0</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="23">
         <f>L4*tax_rate</f>
         <v>0</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="23">
         <f>M4*tax_rate</f>
         <v>0</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="23">
         <f>N4*tax_rate</f>
         <v>0</v>
       </c>
@@ -2602,105 +2317,99 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1">
-        <f>Raw_FS!B$11</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <f>Raw_FS!C$11</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <f>Raw_FS!D$11</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <f>Raw_FS!E$11</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <f>Raw_FS!F$11</f>
-        <v>0</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B6" s="23">
+        <f>Raw_FS!B$5</f>
+        <v>22287000000</v>
+      </c>
+      <c r="C6" s="23">
+        <f>Raw_FS!C$5</f>
+        <v>13861000000</v>
+      </c>
+      <c r="D6" s="23">
+        <f>Raw_FS!D$5</f>
+        <v>14460000000</v>
+      </c>
+      <c r="E6" s="23">
+        <f>Raw_FS!E$5</f>
+        <v>11686000000</v>
+      </c>
+      <c r="F6" s="17"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="1">
+        <v>48</v>
+      </c>
+      <c r="J6" s="23">
         <f>J4-J5</f>
         <v>0</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" ref="K6:N6" si="2">K4-K5</f>
+      <c r="K6" s="23">
+        <f>K4-K5</f>
         <v>0</v>
       </c>
-      <c r="L6" s="1">
-        <f t="shared" si="2"/>
+      <c r="L6" s="23">
+        <f>L4-L5</f>
         <v>0</v>
       </c>
-      <c r="M6" s="1">
-        <f t="shared" si="2"/>
+      <c r="M6" s="23">
+        <f>M4-M5</f>
         <v>0</v>
       </c>
-      <c r="N6" s="1">
-        <f t="shared" si="2"/>
+      <c r="N6" s="23">
+        <f>N4-N5</f>
         <v>0</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1">
-        <f>Raw_FS!B$12</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <f>Raw_FS!C$12</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <f>Raw_FS!D$12</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <f>Raw_FS!E$12</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <f>Raw_FS!F$12</f>
-        <v>0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B7" s="23">
+        <f>B3+B6</f>
+        <v>133009000000</v>
+      </c>
+      <c r="C7" s="23">
+        <f>C3+C6</f>
+        <v>105140000000</v>
+      </c>
+      <c r="D7" s="23">
+        <f>D3+D6</f>
+        <v>100239000000</v>
+      </c>
+      <c r="E7" s="23">
+        <f>E3+E6</f>
+        <v>85134000000</v>
+      </c>
+      <c r="F7" s="17"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="1">
+        <v>50</v>
+      </c>
+      <c r="J7" s="23">
         <f>J2*dep_pct</f>
         <v>0</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="23">
         <f>K2*dep_pct</f>
         <v>0</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="23">
         <f>L2*dep_pct</f>
         <v>0</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="23">
         <f>M2*dep_pct</f>
         <v>0</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="23">
         <f>N2*dep_pct</f>
         <v>0</v>
       </c>
@@ -2708,295 +2417,309 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1">
-        <f>(Raw_FS!B18+Raw_FS!B19-Raw_FS!B20)-(Raw_FS!C18+Raw_FS!C19-Raw_FS!C20)</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <f>(Raw_FS!C18+Raw_FS!C19-Raw_FS!C20)-(Raw_FS!D18+Raw_FS!D19-Raw_FS!D20)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <f>(Raw_FS!D18+Raw_FS!D19-Raw_FS!D20)-(Raw_FS!E18+Raw_FS!E19-Raw_FS!E20)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <f>(Raw_FS!E18+Raw_FS!E19-Raw_FS!E20)-(Raw_FS!F18+Raw_FS!F19-Raw_FS!F20)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <f>(Raw_FS!F18+Raw_FS!F19-Raw_FS!F20)-(Raw_FS!G18+Raw_FS!G19-Raw_FS!G20)</f>
-        <v>0</v>
-      </c>
+    <row r="8" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="21">
+        <f>B7/B2</f>
+        <v>0.54262367310971682</v>
+      </c>
+      <c r="C8" s="21">
+        <f>C7/C2</f>
+        <v>0.49614232121369417</v>
+      </c>
+      <c r="D8" s="21">
+        <f>D7/D2</f>
+        <v>0.50556816462399756</v>
+      </c>
+      <c r="E8" s="21">
+        <f>E7/E2</f>
+        <v>0.50648469849126643</v>
+      </c>
+      <c r="F8" s="17"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="1">
-        <f>J2*capex_pct</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <f>K2*capex_pct</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <f>L2*capex_pct</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="1">
-        <f>M2*capex_pct</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="1">
-        <f>N2*capex_pct</f>
-        <v>0</v>
-      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1">
-        <f>B5+B6-B7-B8</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" ref="C9:F9" si="3">C5+C6-C7-C8</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B9" s="23">
+        <f>Raw_FS!B$12</f>
+        <v>21996000000</v>
+      </c>
+      <c r="C9" s="23">
+        <f>Raw_FS!C$12</f>
+        <v>18095000000</v>
+      </c>
+      <c r="D9" s="23">
+        <f>Raw_FS!D$12</f>
+        <v>19000000000</v>
+      </c>
+      <c r="E9" s="23">
+        <f>Raw_FS!E$12</f>
+        <v>15163000000</v>
+      </c>
+      <c r="F9" s="17"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="1">
-        <f>J2*nwc_pct</f>
+      <c r="I9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="23">
+        <f>J2*capex_pct</f>
         <v>0</v>
       </c>
-      <c r="K9" s="1">
-        <f>K2*nwc_pct</f>
+      <c r="K9" s="23">
+        <f>K2*capex_pct</f>
         <v>0</v>
       </c>
-      <c r="L9" s="1">
-        <f>L2*nwc_pct</f>
+      <c r="L9" s="23">
+        <f>L2*capex_pct</f>
         <v>0</v>
       </c>
-      <c r="M9" s="1">
-        <f>M2*nwc_pct</f>
+      <c r="M9" s="23">
+        <f>M2*capex_pct</f>
         <v>0</v>
       </c>
-      <c r="N9" s="1">
-        <f>N2*nwc_pct</f>
+      <c r="N9" s="23">
+        <f>N2*capex_pct</f>
         <v>0</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="e">
-        <f>B5/(Raw_FS!B$14-Raw_FS!B$2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C10" s="1" t="e">
-        <f>C5/(Raw_FS!C$14-Raw_FS!C$2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10" s="1" t="e">
-        <f>D5/(Raw_FS!D$14-Raw_FS!D$2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" s="1" t="e">
-        <f>E5/(Raw_FS!E$14-Raw_FS!E$2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="1" t="e">
-        <f>F5/(Raw_FS!F$14-Raw_FS!F$2)</f>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="10" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="23">
+        <f>(Raw_FS!B10+Raw_FS!B11-Raw_FS!B12)-(Raw_FS!C10+Raw_FS!C11-Raw_FS!C12)</f>
+        <v>3081000000</v>
+      </c>
+      <c r="C10" s="23">
+        <f>(Raw_FS!C10+Raw_FS!C11-Raw_FS!C12)-(Raw_FS!D10+Raw_FS!D11-Raw_FS!D12)</f>
+        <v>4090000000</v>
+      </c>
+      <c r="D10" s="23">
+        <f>(Raw_FS!D10+Raw_FS!D11-Raw_FS!D12)-(Raw_FS!E10+Raw_FS!E11-Raw_FS!E12)</f>
+        <v>3487000000</v>
+      </c>
+      <c r="E10" s="23">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="17"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="1">
-        <f>J6+J7-J8-J9</f>
+      <c r="I10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="23">
+        <f>J2*nwc_pct</f>
         <v>0</v>
       </c>
-      <c r="K10" s="1">
-        <f t="shared" ref="K10:N10" si="4">K6+K7-K8-K9</f>
+      <c r="K10" s="23">
+        <f>K2*nwc_pct</f>
         <v>0</v>
       </c>
-      <c r="L10" s="1">
-        <f t="shared" si="4"/>
+      <c r="L10" s="23">
+        <f>L2*nwc_pct</f>
         <v>0</v>
       </c>
-      <c r="M10" s="1">
-        <f t="shared" si="4"/>
+      <c r="M10" s="23">
+        <f>M2*nwc_pct</f>
         <v>0</v>
       </c>
-      <c r="N10" s="1">
-        <f t="shared" si="4"/>
+      <c r="N10" s="23">
+        <f>N2*nwc_pct</f>
         <v>0</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="e">
-        <f>B9/B2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C11" s="1" t="e">
-        <f t="shared" ref="C11:F11" si="5">C9/C2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B11" s="23">
+        <f>B5+B6-B9-B10</f>
+        <v>107932000000</v>
+      </c>
+      <c r="C11" s="23">
+        <f>C5+C6-C9-C10</f>
+        <v>82955000000</v>
+      </c>
+      <c r="D11" s="23">
+        <f>D5+D6-D9-D10</f>
+        <v>77752000000</v>
+      </c>
+      <c r="E11" s="23">
+        <f>E5+E6-E9-E10</f>
+        <v>69971000000</v>
+      </c>
+      <c r="F11" s="17"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="1">
-        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="K11" s="1">
-        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="L11" s="1">
-        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="M11" s="1">
-        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
-        <v>1</v>
-      </c>
-      <c r="N11" s="1">
-        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="J11" s="23">
+        <f>J6+J7-J9-J10</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="23">
+        <f>K6+K7-K9-K10</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="23">
+        <f>L6+L7-L9-L10</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="23">
+        <f>M6+M7-M9-M10</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="23">
+        <f>N6+N7-N9-N10</f>
+        <v>0</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="1" t="e">
-        <f>(B2/F2)^(1/4)-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="B12" s="21">
+        <f>B5/(Raw_FS!B$7-Raw_FS!B$9-Raw_FS!B$12)</f>
+        <v>0.23465408645083627</v>
+      </c>
+      <c r="C12" s="21">
+        <f>C5/(Raw_FS!C$7-Raw_FS!C$9-Raw_FS!C$12)</f>
+        <v>0.25413375578057618</v>
+      </c>
+      <c r="D12" s="21">
+        <f>D5/(Raw_FS!D$7-Raw_FS!D$9-Raw_FS!D$12)</f>
+        <v>0.2584413197593316</v>
+      </c>
+      <c r="E12" s="21">
+        <f>E5/(Raw_FS!E$7-Raw_FS!E$9-Raw_FS!E$12)</f>
+        <v>0.24129412073904702</v>
+      </c>
+      <c r="F12" s="17"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="5">
-        <f>J10*J11</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" ref="K12:N12" si="6">K10*K11</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
+      <c r="I12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="23">
+        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="23">
+        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="23">
+        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="23">
+        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="23">
+        <f>1/(1+wacc)^(COLUMN()-COLUMN($J$1)+1)</f>
+        <v>1</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+    <row r="13" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="21">
+        <f>B11/B2</f>
+        <v>0.44031951436427574</v>
+      </c>
+      <c r="C13" s="21">
+        <f>C11/C2</f>
+        <v>0.39145412075596348</v>
+      </c>
+      <c r="D13" s="21">
+        <f>D11/D2</f>
+        <v>0.39215211580168458</v>
+      </c>
+      <c r="E13" s="21">
+        <f>E11/E2</f>
+        <v>0.41627599828661177</v>
+      </c>
+      <c r="F13" s="17"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="17">
-        <f>N$10*(1+Inputs!B16)</f>
+      <c r="I13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="24">
+        <f>J11*J12</f>
         <v>0</v>
       </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="K13" s="24">
+        <f>K11*K12</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="24">
+        <f>L11*L12</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="24">
+        <f>M11*M12</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="24">
+        <f>N11*N12</f>
+        <v>0</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="F14" s="12"/>
-      <c r="I14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="11" t="e">
-        <f>J13/(wacc-Inputs!B16)</f>
-        <v>#DIV/0!</v>
+    <row r="14" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="22">
+        <f>(B2/E2)^(1/3)-1</f>
+        <v>0.13400558612967717</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="18">
+        <f>N$11*(1+Inputs!B16)</f>
+        <v>0</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -3006,18 +2729,18 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="F15" s="12"/>
-      <c r="I15" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J15" s="11">
-        <f>1/(1+wacc)^(COLUMN(N$1)-COLUMN($J$1)+1)</f>
-        <v>1</v>
+      <c r="F15" s="11"/>
+      <c r="I15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="19" t="e">
+        <f>J14/(wacc-Inputs!B16)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -3027,18 +2750,18 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="F16" s="12"/>
-      <c r="I16" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="19" t="e">
-        <f>J14*J15</f>
-        <v>#DIV/0!</v>
+      <c r="F16" s="11"/>
+      <c r="I16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="10">
+        <f>1/(1+wacc)^(COLUMN(N$1)-COLUMN($J$1)+1)</f>
+        <v>1</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -3048,14 +2771,19 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="16.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="F17" s="12"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="F17" s="11"/>
+      <c r="I17" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="20" t="e">
+        <f>J15*J16</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -3064,20 +2792,12 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="1">
-        <f>SUM(J12:N12)</f>
-        <v>0</v>
-      </c>
+    <row r="18" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="F18" s="11"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -3088,18 +2808,20 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="1" t="e">
-        <f>pv_fcff_total+J16</f>
-        <v>#DIV/0!</v>
+        <v>64</v>
+      </c>
+      <c r="B19" s="1">
+        <f>SUM(J13:N13)</f>
+        <v>0</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -3110,13 +2832,13 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="1">
-        <f>Raw_FS!B$17-Raw_FS!B$16</f>
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="B20" s="1" t="e">
+        <f>pv_fcff_total+J17</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -3132,13 +2854,13 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="1" t="e">
-        <f>ev-net_debt</f>
-        <v>#DIV/0!</v>
+        <v>66</v>
+      </c>
+      <c r="B21" s="1">
+        <f>Raw_FS!B$17-Raw_FS!B$16</f>
+        <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -3154,13 +2876,13 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="1">
-        <f>Inputs!B3</f>
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="B22" s="1" t="e">
+        <f>ev-net_debt</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -3176,13 +2898,13 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="1" t="e">
-        <f>equity_value/shares_out</f>
-        <v>#DIV/0!</v>
+        <v>68</v>
+      </c>
+      <c r="B23" s="1">
+        <f>Inputs!B3</f>
+        <v>0</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -3198,11 +2920,14 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="B24" s="1" t="e">
+        <f>equity_value/shares_out</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3217,14 +2942,11 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="1" t="e">
-        <f>implied_price/current_price - 1</f>
-        <v>#DIV/0!</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3239,9 +2961,14 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+    <row r="26" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="1" t="e">
+        <f>implied_price/current_price - 1</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -3256,15 +2983,13 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -3275,7 +3000,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3294,7 +3019,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3313,7 +3038,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3332,7 +3057,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3351,7 +3076,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3370,7 +3095,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3389,7 +3114,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3408,7 +3133,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3427,7 +3152,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3446,7 +3171,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3465,7 +3190,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3484,7 +3209,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3503,7 +3228,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3522,7 +3247,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3541,7 +3266,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3560,7 +3285,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3579,7 +3304,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3598,7 +3323,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3617,7 +3342,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3636,7 +3361,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3655,7 +3380,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3674,7 +3399,7 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
-    <row r="49" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3693,7 +3418,7 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
     </row>
-    <row r="50" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3712,7 +3437,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3731,7 +3456,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3750,7 +3475,7 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3769,7 +3494,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
     </row>
-    <row r="54" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3788,7 +3513,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
     </row>
-    <row r="55" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3807,7 +3532,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
     </row>
-    <row r="56" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3826,7 +3551,7 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
     </row>
-    <row r="57" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3845,7 +3570,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
     </row>
-    <row r="58" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3864,7 +3589,7 @@
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
     </row>
-    <row r="59" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3883,7 +3608,7 @@
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
     </row>
-    <row r="60" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3902,7 +3627,7 @@
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
     </row>
-    <row r="61" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3921,7 +3646,7 @@
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
     </row>
-    <row r="62" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3940,7 +3665,7 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3959,7 +3684,7 @@
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
     </row>
-    <row r="64" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3978,7 +3703,7 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3997,7 +3722,7 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4016,7 +3741,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4035,7 +3760,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4054,7 +3779,7 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4073,7 +3798,7 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4092,7 +3817,7 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4111,7 +3836,7 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4130,7 +3855,7 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4149,7 +3874,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4168,7 +3893,7 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
     </row>
-    <row r="75" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4187,7 +3912,7 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
     </row>
-    <row r="76" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4206,7 +3931,7 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
     </row>
-    <row r="77" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4225,7 +3950,7 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
     </row>
-    <row r="78" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4244,7 +3969,7 @@
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
     </row>
-    <row r="79" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4263,7 +3988,7 @@
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
     </row>
-    <row r="80" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4282,7 +4007,7 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
     </row>
-    <row r="81" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4301,7 +4026,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4320,7 +4045,7 @@
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
     </row>
-    <row r="83" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -4339,7 +4064,7 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4358,7 +4083,7 @@
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
     </row>
-    <row r="85" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4377,7 +4102,7 @@
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
     </row>
-    <row r="86" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -4396,7 +4121,7 @@
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
     </row>
-    <row r="87" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -4415,7 +4140,7 @@
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
     </row>
-    <row r="88" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -4434,7 +4159,7 @@
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
     </row>
-    <row r="89" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -4453,7 +4178,7 @@
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
     </row>
-    <row r="90" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -4472,7 +4197,7 @@
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
     </row>
-    <row r="91" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -4491,7 +4216,7 @@
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
     </row>
-    <row r="92" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -4510,7 +4235,7 @@
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
     </row>
-    <row r="93" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -4529,7 +4254,7 @@
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
     </row>
-    <row r="94" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -4548,7 +4273,7 @@
       <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
     </row>
-    <row r="95" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -4567,7 +4292,7 @@
       <c r="P95" s="1"/>
       <c r="Q95" s="1"/>
     </row>
-    <row r="96" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -4586,7 +4311,7 @@
       <c r="P96" s="1"/>
       <c r="Q96" s="1"/>
     </row>
-    <row r="97" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -4605,7 +4330,7 @@
       <c r="P97" s="1"/>
       <c r="Q97" s="1"/>
     </row>
-    <row r="98" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -4624,7 +4349,7 @@
       <c r="P98" s="1"/>
       <c r="Q98" s="1"/>
     </row>
-    <row r="99" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -4643,7 +4368,7 @@
       <c r="P99" s="1"/>
       <c r="Q99" s="1"/>
     </row>
-    <row r="100" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -4662,7 +4387,7 @@
       <c r="P100" s="1"/>
       <c r="Q100" s="1"/>
     </row>
-    <row r="101" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -4681,7 +4406,7 @@
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
     </row>
-    <row r="102" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4700,7 +4425,7 @@
       <c r="P102" s="1"/>
       <c r="Q102" s="1"/>
     </row>
-    <row r="103" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -4719,7 +4444,7 @@
       <c r="P103" s="1"/>
       <c r="Q103" s="1"/>
     </row>
-    <row r="104" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -4738,7 +4463,7 @@
       <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
     </row>
-    <row r="105" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -4757,7 +4482,7 @@
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
     </row>
-    <row r="106" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -4776,7 +4501,7 @@
       <c r="P106" s="1"/>
       <c r="Q106" s="1"/>
     </row>
-    <row r="107" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -4795,7 +4520,7 @@
       <c r="P107" s="1"/>
       <c r="Q107" s="1"/>
     </row>
-    <row r="108" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -4814,7 +4539,7 @@
       <c r="P108" s="1"/>
       <c r="Q108" s="1"/>
     </row>
-    <row r="109" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -4833,7 +4558,7 @@
       <c r="P109" s="1"/>
       <c r="Q109" s="1"/>
     </row>
-    <row r="110" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -4852,7 +4577,7 @@
       <c r="P110" s="1"/>
       <c r="Q110" s="1"/>
     </row>
-    <row r="111" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -4871,7 +4596,7 @@
       <c r="P111" s="1"/>
       <c r="Q111" s="1"/>
     </row>
-    <row r="112" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -4890,7 +4615,7 @@
       <c r="P112" s="1"/>
       <c r="Q112" s="1"/>
     </row>
-    <row r="113" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -4909,7 +4634,7 @@
       <c r="P113" s="1"/>
       <c r="Q113" s="1"/>
     </row>
-    <row r="114" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -4928,7 +4653,7 @@
       <c r="P114" s="1"/>
       <c r="Q114" s="1"/>
     </row>
-    <row r="115" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -4947,7 +4672,7 @@
       <c r="P115" s="1"/>
       <c r="Q115" s="1"/>
     </row>
-    <row r="116" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -4966,7 +4691,7 @@
       <c r="P116" s="1"/>
       <c r="Q116" s="1"/>
     </row>
-    <row r="117" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -4985,7 +4710,7 @@
       <c r="P117" s="1"/>
       <c r="Q117" s="1"/>
     </row>
-    <row r="118" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -5004,7 +4729,7 @@
       <c r="P118" s="1"/>
       <c r="Q118" s="1"/>
     </row>
-    <row r="119" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -5023,7 +4748,7 @@
       <c r="P119" s="1"/>
       <c r="Q119" s="1"/>
     </row>
-    <row r="120" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -5042,7 +4767,7 @@
       <c r="P120" s="1"/>
       <c r="Q120" s="1"/>
     </row>
-    <row r="121" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -5061,7 +4786,7 @@
       <c r="P121" s="1"/>
       <c r="Q121" s="1"/>
     </row>
-    <row r="122" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -5080,7 +4805,7 @@
       <c r="P122" s="1"/>
       <c r="Q122" s="1"/>
     </row>
-    <row r="123" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -5099,7 +4824,7 @@
       <c r="P123" s="1"/>
       <c r="Q123" s="1"/>
     </row>
-    <row r="124" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -5118,7 +4843,7 @@
       <c r="P124" s="1"/>
       <c r="Q124" s="1"/>
     </row>
-    <row r="125" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -5137,7 +4862,7 @@
       <c r="P125" s="1"/>
       <c r="Q125" s="1"/>
     </row>
-    <row r="126" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -5156,7 +4881,7 @@
       <c r="P126" s="1"/>
       <c r="Q126" s="1"/>
     </row>
-    <row r="127" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -5175,7 +4900,7 @@
       <c r="P127" s="1"/>
       <c r="Q127" s="1"/>
     </row>
-    <row r="128" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -5194,7 +4919,7 @@
       <c r="P128" s="1"/>
       <c r="Q128" s="1"/>
     </row>
-    <row r="129" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -5213,7 +4938,7 @@
       <c r="P129" s="1"/>
       <c r="Q129" s="1"/>
     </row>
-    <row r="130" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -5232,7 +4957,7 @@
       <c r="P130" s="1"/>
       <c r="Q130" s="1"/>
     </row>
-    <row r="131" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -5251,7 +4976,7 @@
       <c r="P131" s="1"/>
       <c r="Q131" s="1"/>
     </row>
-    <row r="132" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -5270,7 +4995,7 @@
       <c r="P132" s="1"/>
       <c r="Q132" s="1"/>
     </row>
-    <row r="133" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -5289,7 +5014,7 @@
       <c r="P133" s="1"/>
       <c r="Q133" s="1"/>
     </row>
-    <row r="134" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -5308,7 +5033,7 @@
       <c r="P134" s="1"/>
       <c r="Q134" s="1"/>
     </row>
-    <row r="135" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -5327,7 +5052,7 @@
       <c r="P135" s="1"/>
       <c r="Q135" s="1"/>
     </row>
-    <row r="136" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -5346,7 +5071,7 @@
       <c r="P136" s="1"/>
       <c r="Q136" s="1"/>
     </row>
-    <row r="137" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -5365,7 +5090,7 @@
       <c r="P137" s="1"/>
       <c r="Q137" s="1"/>
     </row>
-    <row r="138" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -5384,7 +5109,7 @@
       <c r="P138" s="1"/>
       <c r="Q138" s="1"/>
     </row>
-    <row r="139" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -5403,7 +5128,7 @@
       <c r="P139" s="1"/>
       <c r="Q139" s="1"/>
     </row>
-    <row r="140" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -5422,7 +5147,7 @@
       <c r="P140" s="1"/>
       <c r="Q140" s="1"/>
     </row>
-    <row r="141" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -5441,7 +5166,7 @@
       <c r="P141" s="1"/>
       <c r="Q141" s="1"/>
     </row>
-    <row r="142" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -5460,7 +5185,7 @@
       <c r="P142" s="1"/>
       <c r="Q142" s="1"/>
     </row>
-    <row r="143" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -5479,7 +5204,7 @@
       <c r="P143" s="1"/>
       <c r="Q143" s="1"/>
     </row>
-    <row r="144" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -5498,7 +5223,7 @@
       <c r="P144" s="1"/>
       <c r="Q144" s="1"/>
     </row>
-    <row r="145" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -5517,7 +5242,7 @@
       <c r="P145" s="1"/>
       <c r="Q145" s="1"/>
     </row>
-    <row r="146" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -5536,7 +5261,7 @@
       <c r="P146" s="1"/>
       <c r="Q146" s="1"/>
     </row>
-    <row r="147" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -5555,7 +5280,7 @@
       <c r="P147" s="1"/>
       <c r="Q147" s="1"/>
     </row>
-    <row r="148" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -5574,7 +5299,7 @@
       <c r="P148" s="1"/>
       <c r="Q148" s="1"/>
     </row>
-    <row r="149" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -5593,7 +5318,7 @@
       <c r="P149" s="1"/>
       <c r="Q149" s="1"/>
     </row>
-    <row r="150" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -5612,7 +5337,7 @@
       <c r="P150" s="1"/>
       <c r="Q150" s="1"/>
     </row>
-    <row r="151" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -5631,7 +5356,7 @@
       <c r="P151" s="1"/>
       <c r="Q151" s="1"/>
     </row>
-    <row r="152" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -5650,7 +5375,7 @@
       <c r="P152" s="1"/>
       <c r="Q152" s="1"/>
     </row>
-    <row r="153" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -5669,7 +5394,7 @@
       <c r="P153" s="1"/>
       <c r="Q153" s="1"/>
     </row>
-    <row r="154" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -5688,7 +5413,7 @@
       <c r="P154" s="1"/>
       <c r="Q154" s="1"/>
     </row>
-    <row r="155" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -5707,17 +5432,37 @@
       <c r="P155" s="1"/>
       <c r="Q155" s="1"/>
     </row>
+    <row r="156" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+      <c r="N156" s="1"/>
+      <c r="O156" s="1"/>
+      <c r="P156" s="1"/>
+      <c r="Q156" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CA4D06-E805-4423-BAEC-8F1E02BD852C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5725,9 +5470,9 @@
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="e">
         <f>implied_price</f>
@@ -5740,9 +5485,9 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -5752,9 +5497,9 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="e">
         <f>upside_pct</f>
@@ -5767,9 +5512,9 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <f>wacc</f>
@@ -5782,9 +5527,9 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1">
         <f>Inputs!B16</f>
@@ -5797,9 +5542,9 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5809,9 +5554,9 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1">
         <f>Inputs!B18</f>
@@ -5824,7 +5569,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5834,7 +5579,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -5844,7 +5589,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -5854,7 +5599,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -5864,7 +5609,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -5874,7 +5619,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -5884,7 +5629,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -5894,7 +5639,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -5904,7 +5649,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -5914,7 +5659,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -5924,7 +5669,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -5934,7 +5679,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -5944,7 +5689,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -5954,7 +5699,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -5964,7 +5709,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -5976,11 +5721,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$B$3&gt;0</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$B$3&lt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$B$3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>